<commit_message>
fix Not available in create register form
</commit_message>
<xml_diff>
--- a/backend/data/ki1.xlsx
+++ b/backend/data/ki1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SON.admin\VIII\Architecture\credit-based-course-management\backend\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SON.admin\VIII\Architecture\dkhp-iuh-edu-vn\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC4B94A-D5EE-4D35-9967-FF41AC443D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A88D196-256C-47A7-9B52-901B9DBF6BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{02EF117C-553B-4DD7-84CE-F60C11302335}"/>
   </bookViews>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8E1DB4-7413-4561-95DC-BC2E4D393355}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -624,30 +624,30 @@
       </c>
       <c r="E2" s="3" t="str">
         <f ca="1">RANDBETWEEN(10000007,10000015)&amp;""</f>
-        <v>10000011</v>
+        <v>10000015</v>
       </c>
       <c r="F2" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000012,10000013,10000009</v>
+        <v>10000008,10000009,10000013</v>
       </c>
       <c r="G2" s="5">
         <v>45</v>
       </c>
       <c r="H2" s="2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"X1_01", "X1_02", "X1_03", "X1_04", "X1_05","X1_06", "X1_07", "X1_08", "X1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-01-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_7_TO_9,X1_07,2024-01-05T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+        <v>HOUR_4_TO_6,X1_08,2024-01-02T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
       </c>
       <c r="I2" s="2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_10_TO_12,H1_02,2024-02-04T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <v>HOUR_4_TO_6,H1_03,2024-02-03T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
       </c>
       <c r="J2" s="2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_7_TO_9,H1_03,2024-02-02T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+        <v>HOUR_10_TO_12,H1_04,2024-02-03T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
       <c r="K2" s="2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_10_TO_12,H1_09,2024-02-06T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+        <v>HOUR_1_TO_3,H1_02,2024-02-05T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -665,30 +665,30 @@
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" ref="E3:E26" ca="1" si="0">RANDBETWEEN(10000007,10000015)&amp;""</f>
-        <v>10000012</v>
+        <v>10000015</v>
       </c>
       <c r="F3" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000013,10000007,10000007</v>
+        <v>10000014,10000010,10000010</v>
       </c>
       <c r="G3" s="5">
         <v>3</v>
       </c>
       <c r="H3" s="2" t="str">
-        <f t="shared" ref="H2:H4" ca="1" si="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"X1_01", "X1_02", "X1_03", "X1_04", "X1_05","X1_06", "X1_07", "X1_08", "X1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-01-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_4_TO_6,X1_04,2024-01-06T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+        <f ca="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"X1_01", "X1_02", "X1_03", "X1_04", "X1_05","X1_06", "X1_07", "X1_08", "X1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-01-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
+        <v>HOUR_10_TO_12,X1_08,2024-01-01T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I2:K17" ca="1" si="2">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_7_TO_9,H1_02,2024-02-04T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ref="I3:K16" ca="1" si="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
+        <v>HOUR_10_TO_12,H1_06,2024-02-05T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_1_TO_3,H1_01,2024-02-07T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_4_TO_6,H1_05,2024-02-06T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
       </c>
       <c r="K3" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_4_TO_6,H1_06,2024-02-02T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_10_TO_12,H1_09,2024-02-07T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000009</v>
+        <v>10000013</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="5">
@@ -714,7 +714,7 @@
       </c>
       <c r="H4" s="2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"X1_01", "X1_02", "X1_03", "X1_04", "X1_05","X1_06", "X1_07", "X1_08", "X1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-01-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_10_TO_12,X1_01,2024-01-07T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <v>HOUR_4_TO_6,X1_01,2024-01-07T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -735,30 +735,30 @@
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000013</v>
+        <v>10000011</v>
       </c>
       <c r="F5" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000014,10000010,10000012</v>
+        <v>10000007,10000012,10000015</v>
       </c>
       <c r="G5" s="5">
         <v>3</v>
       </c>
       <c r="H5" s="2" t="str">
-        <f t="shared" ref="H5:H12" ca="1" si="3">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"X1_01", "X1_02", "X1_03", "X1_04", "X1_05","X1_06", "X1_07", "X1_08", "X1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-01-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_1_TO_3,X1_06,2024-01-07T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ref="H5:H12" ca="1" si="2">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"X1_01", "X1_02", "X1_03", "X1_04", "X1_05","X1_06", "X1_07", "X1_08", "X1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-01-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
+        <v>HOUR_4_TO_6,X1_08,2024-01-07T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
       </c>
       <c r="I5" s="2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_7_TO_9,H1_04,2024-02-06T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+        <v>HOUR_4_TO_6,H1_06,2024-02-04T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
       </c>
       <c r="J5" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_7_TO_9,H1_08,2024-02-03T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_7_TO_9,H1_02,2024-02-07T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
       </c>
       <c r="K5" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_7_TO_9,H1_08,2024-02-02T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_4_TO_6,H1_09,2024-02-01T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -776,30 +776,30 @@
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000013</v>
+        <v>10000007</v>
       </c>
       <c r="F6" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000010,10000010,10000009</v>
+        <v>10000013,10000010,10000015</v>
       </c>
       <c r="G6" s="5">
         <v>3</v>
       </c>
       <c r="H6" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>HOUR_1_TO_3,X1_02,2024-01-05T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>HOUR_7_TO_9,X1_01,2024-01-03T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
       <c r="I6" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_7_TO_9,H1_02,2024-02-03T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_4_TO_6,H1_06,2024-02-04T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_1_TO_3,H1_08,2024-02-04T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_4_TO_6,H1_02,2024-02-04T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
       </c>
       <c r="K6" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_4_TO_6,H1_03,2024-02-04T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_7_TO_9,H1_04,2024-02-01T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -817,30 +817,30 @@
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000007</v>
+        <v>10000013</v>
       </c>
       <c r="F7" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000010,10000008,10000013</v>
+        <v>10000009,10000011,10000015</v>
       </c>
       <c r="G7" s="5">
         <v>3</v>
       </c>
       <c r="H7" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>HOUR_7_TO_9,X1_05,2024-01-07T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>HOUR_4_TO_6,X1_06,2024-01-06T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
       </c>
       <c r="I7" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_4_TO_6,H1_07,2024-02-03T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_10_TO_12,H1_05,2024-02-01T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
       <c r="J7" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_7_TO_9,H1_02,2024-02-07T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f ca="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
+        <v>HOUR_1_TO_3,H1_08,2024-02-07T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
       </c>
       <c r="K7" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_7_TO_9,H1_05,2024-02-06T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_7_TO_9,H1_06,2024-02-05T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -865,17 +865,17 @@
         <v>3</v>
       </c>
       <c r="H8" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>HOUR_1_TO_3,X1_03,2024-01-06T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>HOUR_4_TO_6,X1_08,2024-01-04T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_4_TO_6,H1_03,2024-02-04T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_4_TO_6,H1_05,2024-02-01T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
       </c>
       <c r="K8" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_4_TO_6,H1_06,2024-02-04T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_1_TO_3,H1_05,2024-02-06T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -893,30 +893,30 @@
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000009</v>
+        <v>10000013</v>
       </c>
       <c r="F9" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000012,10000014,10000013</v>
+        <v>10000009,10000015,10000015</v>
       </c>
       <c r="G9" s="5">
         <v>45</v>
       </c>
       <c r="H9" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>HOUR_10_TO_12,X1_03,2024-01-07T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>HOUR_7_TO_9,X1_03,2024-01-07T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
       </c>
       <c r="I9" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_10_TO_12,H1_03,2024-02-06T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_4_TO_6,H1_04,2024-02-06T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
       </c>
       <c r="J9" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_4_TO_6,H1_09,2024-02-05T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_1_TO_3,H1_08,2024-02-02T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
       </c>
       <c r="K9" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_10_TO_12,H1_09,2024-02-04T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_10_TO_12,H1_04,2024-02-04T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -934,30 +934,30 @@
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000014</v>
+        <v>10000015</v>
       </c>
       <c r="F10" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000015,10000014,10000011</v>
+        <v>10000011,10000011,10000013</v>
       </c>
       <c r="G10" s="5">
         <v>3</v>
       </c>
       <c r="H10" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>HOUR_7_TO_9,X1_03,2024-01-05T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>HOUR_10_TO_12,X1_06,2024-01-01T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
       </c>
       <c r="I10" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_4_TO_6,H1_05,2024-02-07T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_10_TO_12,H1_05,2024-02-05T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
       </c>
       <c r="J10" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_10_TO_12,H1_08,2024-02-01T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_10_TO_12,H1_02,2024-02-06T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
       </c>
       <c r="K10" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_4_TO_6,H1_07,2024-02-03T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_4_TO_6,H1_09,2024-02-05T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -975,15 +975,15 @@
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000012</v>
+        <v>10000007</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="5">
         <v>3</v>
       </c>
       <c r="H11" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>HOUR_4_TO_6,X1_09,2024-01-07T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>HOUR_10_TO_12,X1_02,2024-01-07T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1004,15 +1004,15 @@
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000010</v>
+        <v>10000012</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="5">
         <v>3</v>
       </c>
       <c r="H12" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>HOUR_7_TO_9,X1_07,2024-01-04T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>HOUR_4_TO_6,X1_06,2024-01-02T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1033,15 +1033,15 @@
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000011</v>
+        <v>10000015</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="5">
         <v>3</v>
       </c>
       <c r="H13" s="2" t="str">
-        <f t="shared" ref="H6:H26" ca="1" si="4">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"X1_01", "X1_02", "X1_03", "X1_04", "X1_05","X1_06", "X1_07", "X1_08", "X1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-01-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_7_TO_9,X1_05,2024-01-05T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f t="shared" ref="H13:H26" ca="1" si="3">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"X1_01", "X1_02", "X1_03", "X1_04", "X1_05","X1_06", "X1_07", "X1_08", "X1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-01-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
+        <v>HOUR_10_TO_12,X1_02,2024-01-07T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1062,15 +1062,15 @@
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000010</v>
+        <v>10000007</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="5">
         <v>3</v>
       </c>
       <c r="H14" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>HOUR_7_TO_9,X1_07,2024-01-03T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_7_TO_9,X1_08,2024-01-01T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1091,15 +1091,15 @@
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000015</v>
+        <v>10000014</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="5">
         <v>3</v>
       </c>
       <c r="H15" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>HOUR_4_TO_6,X1_03,2024-01-01T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_4_TO_6,X1_08,2024-01-05T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1120,30 +1120,30 @@
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000014</v>
+        <v>10000015</v>
       </c>
       <c r="F16" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000009,10000009,10000013</v>
+        <v>10000009,10000013,10000010</v>
       </c>
       <c r="G16" s="5">
         <v>3</v>
       </c>
       <c r="H16" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>HOUR_4_TO_6,X1_02,2024-01-07T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_1_TO_3,X1_07,2024-01-02T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
       </c>
       <c r="I16" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_1_TO_3,H1_03,2024-02-04T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_1_TO_3,H1_06,2024-02-07T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
       </c>
       <c r="J16" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_1_TO_3,H1_01,2024-02-01T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_4_TO_6,H1_05,2024-02-01T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
       </c>
       <c r="K16" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>HOUR_4_TO_6,H1_06,2024-02-04T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>HOUR_1_TO_3,H1_03,2024-02-02T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1161,15 +1161,15 @@
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000010</v>
+        <v>10000009</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="5">
         <v>3</v>
       </c>
       <c r="H17" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>HOUR_1_TO_3,X1_08,2024-01-01T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_1_TO_3,X1_05,2024-01-07T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1197,8 +1197,8 @@
         <v>3</v>
       </c>
       <c r="H18" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>HOUR_10_TO_12,X1_02,2024-01-04T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_10_TO_12,X1_09,2024-01-02T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1219,30 +1219,30 @@
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000015</v>
+        <v>10000008</v>
       </c>
       <c r="F19" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000008,10000011,10000009</v>
+        <v>10000010,10000012,10000011</v>
       </c>
       <c r="G19" s="5">
         <v>45</v>
       </c>
       <c r="H19" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>HOUR_7_TO_9,X1_07,2024-01-01T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_1_TO_3,X1_04,2024-01-02T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
       <c r="I19" s="2" t="str">
-        <f t="shared" ref="I18:I26" ca="1" si="5">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_10_TO_12,H1_05,2024-02-04T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <f t="shared" ref="I19:I26" ca="1" si="4">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
+        <v>HOUR_7_TO_9,H1_04,2024-02-07T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f t="shared" ref="J18:J26" ca="1" si="6">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_7_TO_9,H1_02,2024-02-02T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
+        <f t="shared" ref="J19:J26" ca="1" si="5">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
+        <v>HOUR_10_TO_12,H1_01,2024-02-01T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
       </c>
       <c r="K19" s="2" t="str">
-        <f t="shared" ref="K18:K26" ca="1" si="7">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
-        <v>HOUR_10_TO_12,H1_03,2024-02-02T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+        <f t="shared" ref="K19:K26" ca="1" si="6">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
+        <v>HOUR_10_TO_12,H1_09,2024-02-02T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1260,30 +1260,30 @@
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000011</v>
+        <v>10000008</v>
       </c>
       <c r="F20" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000010,10000015,10000009</v>
+        <v>10000009,10000014,10000015</v>
       </c>
       <c r="G20" s="5">
         <v>3</v>
       </c>
       <c r="H20" s="2" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_7_TO_9,X1_07,2024-01-06T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+      </c>
+      <c r="I20" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>HOUR_7_TO_9,X1_08,2024-01-05T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
-      </c>
-      <c r="I20" s="2" t="str">
+        <v>HOUR_7_TO_9,H1_05,2024-02-05T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+      </c>
+      <c r="J20" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HOUR_10_TO_12,H1_09,2024-02-02T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
-      </c>
-      <c r="J20" s="2" t="str">
+        <v>HOUR_10_TO_12,H1_04,2024-02-02T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+      </c>
+      <c r="K20" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HOUR_7_TO_9,H1_01,2024-02-02T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
-      </c>
-      <c r="K20" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>HOUR_7_TO_9,H1_03,2024-02-06T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
+        <v>HOUR_4_TO_6,H1_06,2024-02-06T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1301,15 +1301,15 @@
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000013</v>
+        <v>10000012</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="5">
         <v>3</v>
       </c>
       <c r="H21" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>HOUR_4_TO_6,X1_09,2024-01-05T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_7_TO_9,X1_08,2024-01-04T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1337,8 +1337,8 @@
         <v>3</v>
       </c>
       <c r="H22" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>HOUR_7_TO_9,X1_09,2024-01-03T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_7_TO_9,X1_09,2024-01-06T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1359,30 +1359,30 @@
       </c>
       <c r="E23" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000008</v>
+        <v>10000012</v>
       </c>
       <c r="F23" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000012,10000008,10000008</v>
+        <v>10000009,10000011,10000013</v>
       </c>
       <c r="G23" s="5">
         <v>45</v>
       </c>
       <c r="H23" s="2" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_7_TO_9,X1_05,2024-01-02T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+      </c>
+      <c r="I23" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>HOUR_4_TO_6,X1_08,2024-01-05T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
-      </c>
-      <c r="I23" s="2" t="str">
+        <v>HOUR_4_TO_6,H1_09,2024-02-02T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+      </c>
+      <c r="J23" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HOUR_7_TO_9,H1_01,2024-02-07T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
-      </c>
-      <c r="J23" s="2" t="str">
+        <v>HOUR_1_TO_3,H1_08,2024-02-07T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+      </c>
+      <c r="K23" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HOUR_10_TO_12,H1_09,2024-02-02T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
-      </c>
-      <c r="K23" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>HOUR_7_TO_9,H1_03,2024-02-05T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <v>HOUR_7_TO_9,H1_01,2024-02-05T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1400,30 +1400,30 @@
       </c>
       <c r="E24" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000009</v>
+        <v>10000014</v>
       </c>
       <c r="F24" s="2" t="str">
         <f ca="1">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000007,10000009,10000014</v>
+        <v>10000014,10000008,10000010</v>
       </c>
       <c r="G24" s="5">
         <v>3</v>
       </c>
       <c r="H24" s="2" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_10_TO_12,X1_03,2024-01-05T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+      </c>
+      <c r="I24" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>HOUR_1_TO_3,X1_09,2024-01-01T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
-      </c>
-      <c r="I24" s="2" t="str">
+        <v>HOUR_1_TO_3,H1_06,2024-02-01T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+      </c>
+      <c r="J24" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HOUR_1_TO_3,H1_02,2024-02-06T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
-      </c>
-      <c r="J24" s="2" t="str">
+        <v>HOUR_1_TO_3,H1_01,2024-02-06T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
+      </c>
+      <c r="K24" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HOUR_4_TO_6,H1_08,2024-02-03T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
-      </c>
-      <c r="K24" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>HOUR_4_TO_6,H1_04,2024-02-02T00:00:00.000Z,2024-04-04T00:00:00.000Z</v>
+        <v>HOUR_4_TO_6,H1_05,2024-02-04T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1441,30 +1441,30 @@
       </c>
       <c r="E25" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10000008</v>
+        <v>10000012</v>
       </c>
       <c r="F25" s="2" t="str">
-        <f t="shared" ref="F25:F26" ca="1" si="8">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
-        <v>10000008,10000014,10000011</v>
+        <f t="shared" ref="F25:F26" ca="1" si="7">RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015) &amp; "," &amp; RANDBETWEEN(10000007, 10000015)</f>
+        <v>10000009,10000009,10000012</v>
       </c>
       <c r="G25" s="5">
         <v>45</v>
       </c>
       <c r="H25" s="2" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_1_TO_3,X1_01,2024-01-01T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+      </c>
+      <c r="I25" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>HOUR_4_TO_6,X1_02,2024-01-07T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
-      </c>
-      <c r="I25" s="2" t="str">
+        <v>HOUR_4_TO_6,H1_03,2024-02-01T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+      </c>
+      <c r="J25" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HOUR_10_TO_12,H1_06,2024-02-01T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
-      </c>
-      <c r="J25" s="2" t="str">
+        <v>HOUR_10_TO_12,H1_06,2024-02-01T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
+      </c>
+      <c r="K25" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HOUR_7_TO_9,H1_02,2024-02-06T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
-      </c>
-      <c r="K25" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>HOUR_4_TO_6,H1_05,2024-02-02T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
+        <v>HOUR_4_TO_6,H1_08,2024-02-04T00:00:00.000Z,2024-04-05T00:00:00.000Z</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1485,27 +1485,27 @@
         <v>10000009</v>
       </c>
       <c r="F26" s="2" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v>10000013,10000009,10000014</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>10000009,10000008,10000015</v>
       </c>
       <c r="G26" s="5">
         <v>3</v>
       </c>
       <c r="H26" s="2" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>HOUR_10_TO_12,X1_01,2024-01-03T00:00:00.000Z,2024-04-03T00:00:00.000Z</v>
+      </c>
+      <c r="I26" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>HOUR_4_TO_6,X1_02,2024-01-06T00:00:00.000Z,2024-04-01T00:00:00.000Z</v>
-      </c>
-      <c r="I26" s="2" t="str">
+        <v>HOUR_4_TO_6,H1_06,2024-02-07T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+      </c>
+      <c r="J26" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HOUR_4_TO_6,H1_07,2024-02-02T00:00:00.000Z,2024-04-06T00:00:00.000Z</v>
-      </c>
-      <c r="J26" s="2" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>HOUR_4_TO_6,H1_02,2024-02-03T00:00:00.000Z,2024-04-07T00:00:00.000Z</v>
+        <v>HOUR_1_TO_3,H1_09,2024-02-02T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
       </c>
       <c r="K26" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>HOUR_7_TO_9,H1_09,2024-02-02T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
+        <f ca="1">CHOOSE(RANDBETWEEN(1,4),"HOUR_1_TO_3","HOUR_4_TO_6","HOUR_7_TO_9","HOUR_10_TO_12")&amp; "," &amp;CHOOSE(RANDBETWEEN(1,9),"H1_01", "H1_02", "H1_03", "H1_04", "H1_05","H1_06", "H1_07", "H1_08", "H1_09")&amp; "," &amp;TEXT(DATEVALUE("2024-02-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")&amp; "," &amp;TEXT(DATEVALUE("2024-04-01") + RANDBETWEEN(0,6), "yyyy-mm-dd\Thh:mm:ss.000\Z")</f>
+        <v>HOUR_4_TO_6,H1_09,2024-02-05T00:00:00.000Z,2024-04-02T00:00:00.000Z</v>
       </c>
     </row>
   </sheetData>

</xml_diff>